<commit_message>
Add fuel_params sheet to input template file.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_template.xlsx
+++ b/co2mpas/co2mpas_template.xlsx
@@ -15,13 +15,14 @@
     <sheet name="gear_box_ratios" sheetId="2" r:id="rId6"/>
     <sheet name="T1_map" sheetId="6" r:id="rId7"/>
     <sheet name="velocity_speed_ratios" sheetId="11" r:id="rId8"/>
+    <sheet name="fuel_params" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="309">
   <si>
     <t>fuel</t>
   </si>
@@ -916,6 +917,39 @@
   <si>
     <t>Start-stop activation time threshold, currently not used by the model to be enabled at future releases</t>
   </si>
+  <si>
+    <t>Param Name</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>l2</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>trg</t>
+  </si>
+  <si>
+    <t>#fuel_params!A2:B_:["dict"]</t>
+  </si>
 </sst>
 </file>
 
@@ -1615,7 +1649,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2773,13 +2827,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" style="43" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="43" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" style="43" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" style="60" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="65" bestFit="1" customWidth="1"/>
@@ -3409,7 +3465,9 @@
       <c r="B30" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="55"/>
+      <c r="C30" s="67" t="s">
+        <v>308</v>
+      </c>
       <c r="D30" s="46" t="s">
         <v>4</v>
       </c>
@@ -4602,58 +4660,68 @@
       <c r="F95" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="C75 C89:C94 C77:C87">
-    <cfRule type="expression" dxfId="10" priority="80">
+    <cfRule type="expression" dxfId="12" priority="82">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C7 C25 C9 C11 C61:C72">
-    <cfRule type="expression" dxfId="9" priority="92">
+    <cfRule type="expression" dxfId="11" priority="94">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58 C14:C16 C8 C10 C27:C31 C21 C23 C18:C19">
-    <cfRule type="expression" dxfId="8" priority="95">
+  <conditionalFormatting sqref="C57:C58 C14:C16 C8 C10 C27:C29 C21 C23 C18:C19 C31">
+    <cfRule type="expression" dxfId="10" priority="97">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15 C3:C6 C61:C72">
-    <cfRule type="expression" dxfId="7" priority="101">
+    <cfRule type="expression" dxfId="9" priority="103">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58 C14:C16 C7:C11 C27:C31 C21 C25 C23 C18:C19">
-    <cfRule type="expression" dxfId="6" priority="105">
+  <conditionalFormatting sqref="C57:C58 C14:C16 C7:C11 C27:C29 C21 C25 C23 C18:C19 C31">
+    <cfRule type="expression" dxfId="8" priority="107">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C34">
-    <cfRule type="expression" dxfId="5" priority="12">
+    <cfRule type="expression" dxfId="7" priority="14">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C34">
-    <cfRule type="expression" dxfId="4" priority="13">
+    <cfRule type="expression" dxfId="6" priority="15">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>#REF!=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>AND(#REF!=1,#REF!=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
+  <conditionalFormatting sqref="C26">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
+  <conditionalFormatting sqref="C30">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
+  <conditionalFormatting sqref="C30">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
@@ -39649,4 +39717,88 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="72"/>
+      <c r="B11" s="72"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
template, #72: Remove target label from NEDC times and velocities inputs.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_template.xlsx
+++ b/co2mpas/co2mpas_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="24645" windowHeight="15300"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="24645" windowHeight="15300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="334">
   <si>
     <t>fuel</t>
   </si>
@@ -840,12 +840,6 @@
   </si>
   <si>
     <t>[km/(h*RPM)]</t>
-  </si>
-  <si>
-    <t>target velocities</t>
-  </si>
-  <si>
-    <t>target times</t>
   </si>
   <si>
     <t>target gears</t>
@@ -1829,17 +1823,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="237">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="123">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1877,66 +1861,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3016,7 +2940,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3037,1076 +2961,6 @@
       <fill>
         <patternFill>
           <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4759,6 +3613,88 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>* May improve the accuracy of MT vehicles if RPM signal or gear ratios values are not very accurate (still under investigation).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7858125" y="581025"/>
+          <a:ext cx="3533775" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE"/>
+            <a:t>SIGN</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" baseline="0"/>
+            <a:t> CONVENTION: t</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE"/>
+            <a:t>he current is negative when is flowing out from the device and positive otherwise.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-IE"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-IE"/>
+            <a:t> </a:t>
           </a:r>
           <a:endParaRPr lang="en-IE">
             <a:effectLst/>
@@ -5691,7 +4627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -5732,10 +4668,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B2" s="77" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C2" s="62">
         <v>2</v>
@@ -5750,7 +4686,7 @@
         <v>43</v>
       </c>
       <c r="G2" s="93" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5771,7 +4707,7 @@
         <v>44</v>
       </c>
       <c r="G3" s="87" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H3" s="35"/>
     </row>
@@ -6004,7 +4940,7 @@
         <v>44</v>
       </c>
       <c r="G14" s="87" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6067,7 +5003,7 @@
         <v>44</v>
       </c>
       <c r="G17" s="87" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6109,15 +5045,15 @@
         <v>44</v>
       </c>
       <c r="G19" s="87" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="78" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="54" t="s">
         <v>305</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>307</v>
       </c>
       <c r="C20" s="74"/>
       <c r="D20" s="84" t="s">
@@ -6130,15 +5066,15 @@
         <v>43</v>
       </c>
       <c r="G20" s="87" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="B21" s="54" t="s">
         <v>306</v>
-      </c>
-      <c r="B21" s="54" t="s">
-        <v>308</v>
       </c>
       <c r="C21" s="74"/>
       <c r="D21" s="84" t="s">
@@ -6151,15 +5087,15 @@
         <v>43</v>
       </c>
       <c r="G21" s="87" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C22" s="74"/>
       <c r="D22" s="84" t="s">
@@ -6172,7 +5108,7 @@
         <v>43</v>
       </c>
       <c r="G22" s="87" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6193,7 +5129,7 @@
         <v>43</v>
       </c>
       <c r="G23" s="87" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6205,7 +5141,7 @@
       </c>
       <c r="C24" s="73"/>
       <c r="D24" s="84" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E24" s="85" t="s">
         <v>214</v>
@@ -6344,7 +5280,7 @@
         <v>45</v>
       </c>
       <c r="G30" s="87" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6365,7 +5301,7 @@
         <v>92</v>
       </c>
       <c r="G31" s="87" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6420,7 +5356,7 @@
         <v>113</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D34" s="84" t="s">
         <v>4</v>
@@ -6974,7 +5910,7 @@
         <v>255</v>
       </c>
       <c r="B61" s="55" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C61" s="70"/>
       <c r="D61" s="84" t="s">
@@ -6987,7 +5923,7 @@
         <v>43</v>
       </c>
       <c r="G61" s="87" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -6995,7 +5931,7 @@
         <v>256</v>
       </c>
       <c r="B62" s="55" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C62" s="70"/>
       <c r="D62" s="84" t="s">
@@ -7008,7 +5944,7 @@
         <v>43</v>
       </c>
       <c r="G62" s="87" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -7029,7 +5965,7 @@
         <v>43</v>
       </c>
       <c r="G63" s="87" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -7496,10 +6432,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="79" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B88" s="55" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C88" s="83"/>
       <c r="D88" s="84" t="s">
@@ -7512,7 +6448,7 @@
         <v>43</v>
       </c>
       <c r="G88" s="87" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -7562,7 +6498,7 @@
         <v>64</v>
       </c>
       <c r="B91" s="55" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C91" s="83"/>
       <c r="D91" s="84" t="s">
@@ -7583,7 +6519,7 @@
         <v>68</v>
       </c>
       <c r="B92" s="55" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C92" s="83"/>
       <c r="D92" s="84" t="s">
@@ -7647,617 +6583,617 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="C79 C94:C99 C81:C92">
-    <cfRule type="expression" dxfId="236" priority="199">
+    <cfRule type="expression" dxfId="122" priority="199">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:C76">
-    <cfRule type="expression" dxfId="235" priority="211">
+    <cfRule type="expression" dxfId="121" priority="211">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:C62 C33 C35">
-    <cfRule type="expression" dxfId="234" priority="214">
+    <cfRule type="expression" dxfId="120" priority="214">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:C76">
-    <cfRule type="expression" dxfId="233" priority="220">
+    <cfRule type="expression" dxfId="119" priority="220">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:C62 C33 C35">
-    <cfRule type="expression" dxfId="232" priority="224">
+    <cfRule type="expression" dxfId="118" priority="224">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C38">
-    <cfRule type="expression" dxfId="231" priority="131">
+    <cfRule type="expression" dxfId="117" priority="131">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C38">
-    <cfRule type="expression" dxfId="230" priority="132">
+    <cfRule type="expression" dxfId="116" priority="132">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="229" priority="122">
+    <cfRule type="expression" dxfId="115" priority="122">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="228" priority="123">
+    <cfRule type="expression" dxfId="114" priority="123">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="225" priority="118">
+    <cfRule type="expression" dxfId="113" priority="118">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="224" priority="119">
+    <cfRule type="expression" dxfId="112" priority="119">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="221" priority="11">
+    <cfRule type="expression" dxfId="111" priority="11">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="219" priority="1">
+    <cfRule type="expression" dxfId="110" priority="1">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10 C4:C8 C12">
-    <cfRule type="expression" dxfId="116" priority="114">
+    <cfRule type="expression" dxfId="109" priority="114">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9 C11">
-    <cfRule type="expression" dxfId="115" priority="115">
+    <cfRule type="expression" dxfId="108" priority="115">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C7">
-    <cfRule type="expression" dxfId="114" priority="116">
+    <cfRule type="expression" dxfId="107" priority="116">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C12">
-    <cfRule type="expression" dxfId="113" priority="117">
+    <cfRule type="expression" dxfId="106" priority="117">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="112" priority="113">
+    <cfRule type="expression" dxfId="105" priority="113">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="111" priority="112">
+    <cfRule type="expression" dxfId="104" priority="112">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="110" priority="111">
+    <cfRule type="expression" dxfId="103" priority="111">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="109" priority="110">
+    <cfRule type="expression" dxfId="102" priority="110">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="108" priority="109">
+    <cfRule type="expression" dxfId="101" priority="109">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="107" priority="108">
+    <cfRule type="expression" dxfId="100" priority="108">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="106" priority="107">
+    <cfRule type="expression" dxfId="99" priority="107">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="105" priority="106">
+    <cfRule type="expression" dxfId="98" priority="106">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="104" priority="105">
+    <cfRule type="expression" dxfId="97" priority="105">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="103" priority="104">
+    <cfRule type="expression" dxfId="96" priority="104">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="102" priority="103">
+    <cfRule type="expression" dxfId="95" priority="103">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="101" priority="102">
+    <cfRule type="expression" dxfId="94" priority="102">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="100" priority="101">
+    <cfRule type="expression" dxfId="93" priority="101">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="99" priority="99">
+    <cfRule type="expression" dxfId="92" priority="99">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="98" priority="100">
+    <cfRule type="expression" dxfId="91" priority="100">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="97" priority="98">
+    <cfRule type="expression" dxfId="90" priority="98">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="96" priority="97">
+    <cfRule type="expression" dxfId="89" priority="97">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="95" priority="96">
+    <cfRule type="expression" dxfId="88" priority="96">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="94" priority="94">
+    <cfRule type="expression" dxfId="87" priority="94">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="93" priority="95">
+    <cfRule type="expression" dxfId="86" priority="95">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="92" priority="93">
+    <cfRule type="expression" dxfId="85" priority="93">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="91" priority="92">
+    <cfRule type="expression" dxfId="84" priority="92">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="90" priority="91">
+    <cfRule type="expression" dxfId="83" priority="91">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="89" priority="89">
+    <cfRule type="expression" dxfId="82" priority="89">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="88" priority="90">
+    <cfRule type="expression" dxfId="81" priority="90">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="87" priority="88">
+    <cfRule type="expression" dxfId="80" priority="88">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="86" priority="87">
+    <cfRule type="expression" dxfId="79" priority="87">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="85" priority="86">
+    <cfRule type="expression" dxfId="78" priority="86">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="84" priority="84">
+    <cfRule type="expression" dxfId="77" priority="84">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="83" priority="85">
+    <cfRule type="expression" dxfId="76" priority="85">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="82" priority="83">
+    <cfRule type="expression" dxfId="75" priority="83">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="81" priority="82">
+    <cfRule type="expression" dxfId="74" priority="82">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="80" priority="81">
+    <cfRule type="expression" dxfId="73" priority="81">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="79" priority="79">
+    <cfRule type="expression" dxfId="72" priority="79">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="78" priority="80">
+    <cfRule type="expression" dxfId="71" priority="80">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="77" priority="78">
+    <cfRule type="expression" dxfId="70" priority="78">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="76" priority="77">
+    <cfRule type="expression" dxfId="69" priority="77">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="75" priority="76">
+    <cfRule type="expression" dxfId="68" priority="76">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="74" priority="74">
+    <cfRule type="expression" dxfId="67" priority="74">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="73" priority="75">
+    <cfRule type="expression" dxfId="66" priority="75">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="72" priority="73">
+    <cfRule type="expression" dxfId="65" priority="73">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="71" priority="72">
+    <cfRule type="expression" dxfId="64" priority="72">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="70" priority="71">
+    <cfRule type="expression" dxfId="63" priority="71">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="69" priority="69">
+    <cfRule type="expression" dxfId="62" priority="69">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="68" priority="70">
+    <cfRule type="expression" dxfId="61" priority="70">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="67" priority="68">
+    <cfRule type="expression" dxfId="60" priority="68">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="66" priority="67">
+    <cfRule type="expression" dxfId="59" priority="67">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="65" priority="66">
+    <cfRule type="expression" dxfId="58" priority="66">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="64" priority="34">
+    <cfRule type="expression" dxfId="57" priority="34">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="63" priority="35">
+    <cfRule type="expression" dxfId="56" priority="35">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="62" priority="33">
+    <cfRule type="expression" dxfId="55" priority="33">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="61" priority="32">
+    <cfRule type="expression" dxfId="54" priority="32">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="60" priority="31">
+    <cfRule type="expression" dxfId="53" priority="31">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="59" priority="64">
+    <cfRule type="expression" dxfId="52" priority="64">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="58" priority="65">
+    <cfRule type="expression" dxfId="51" priority="65">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="57" priority="63">
+    <cfRule type="expression" dxfId="50" priority="63">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="56" priority="62">
+    <cfRule type="expression" dxfId="49" priority="62">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="55" priority="61">
+    <cfRule type="expression" dxfId="48" priority="61">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="54" priority="59">
+    <cfRule type="expression" dxfId="47" priority="59">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="53" priority="60">
+    <cfRule type="expression" dxfId="46" priority="60">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="52" priority="58">
+    <cfRule type="expression" dxfId="45" priority="58">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="51" priority="57">
+    <cfRule type="expression" dxfId="44" priority="57">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="50" priority="56">
+    <cfRule type="expression" dxfId="43" priority="56">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="49" priority="24">
+    <cfRule type="expression" dxfId="42" priority="24">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="48" priority="25">
+    <cfRule type="expression" dxfId="41" priority="25">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="47" priority="23">
+    <cfRule type="expression" dxfId="40" priority="23">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="46" priority="22">
+    <cfRule type="expression" dxfId="39" priority="22">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="45" priority="21">
+    <cfRule type="expression" dxfId="38" priority="21">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="44" priority="54">
+    <cfRule type="expression" dxfId="37" priority="54">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="43" priority="55">
+    <cfRule type="expression" dxfId="36" priority="55">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="42" priority="53">
+    <cfRule type="expression" dxfId="35" priority="53">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="41" priority="52">
+    <cfRule type="expression" dxfId="34" priority="52">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="40" priority="51">
+    <cfRule type="expression" dxfId="33" priority="51">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="39" priority="49">
+    <cfRule type="expression" dxfId="32" priority="49">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="38" priority="50">
+    <cfRule type="expression" dxfId="31" priority="50">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="37" priority="48">
+    <cfRule type="expression" dxfId="30" priority="48">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="36" priority="47">
+    <cfRule type="expression" dxfId="29" priority="47">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="35" priority="46">
+    <cfRule type="expression" dxfId="28" priority="46">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="34" priority="44">
+    <cfRule type="expression" dxfId="27" priority="44">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="33" priority="45">
+    <cfRule type="expression" dxfId="26" priority="45">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="32" priority="43">
+    <cfRule type="expression" dxfId="25" priority="43">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="31" priority="42">
+    <cfRule type="expression" dxfId="24" priority="42">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="30" priority="41">
+    <cfRule type="expression" dxfId="23" priority="41">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="29" priority="39">
+    <cfRule type="expression" dxfId="22" priority="39">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="28" priority="40">
+    <cfRule type="expression" dxfId="21" priority="40">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="27" priority="38">
+    <cfRule type="expression" dxfId="20" priority="38">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="26" priority="37">
+    <cfRule type="expression" dxfId="19" priority="37">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="25" priority="36">
+    <cfRule type="expression" dxfId="18" priority="36">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="24" priority="29">
+    <cfRule type="expression" dxfId="17" priority="29">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="23" priority="30">
+    <cfRule type="expression" dxfId="16" priority="30">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="22" priority="28">
+    <cfRule type="expression" dxfId="15" priority="28">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="21" priority="27">
+    <cfRule type="expression" dxfId="14" priority="27">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="20" priority="26">
+    <cfRule type="expression" dxfId="13" priority="26">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="19" priority="19">
+    <cfRule type="expression" dxfId="12" priority="19">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="18" priority="20">
+    <cfRule type="expression" dxfId="11" priority="20">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="10" priority="18">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="9" priority="17">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>AND(#REF!=0,#REF!=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="7" priority="14">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="6" priority="15">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="5" priority="13">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>AND(#REF!=1,#REF!=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8271,7 +7207,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8288,7 +7226,7 @@
         <v>67</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>65</v>
@@ -8309,7 +7247,7 @@
         <v>66</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>64</v>
@@ -8320,45 +7258,45 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="56" t="s">
+        <v>310</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="J2" s="56" t="s">
-        <v>312</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>280</v>
-      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
       <c r="E3" s="31"/>
@@ -8371,8 +7309,8 @@
       <c r="L3" s="31"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -8385,8 +7323,8 @@
       <c r="L4" s="31"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -8399,8 +7337,8 @@
       <c r="L5" s="31"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="63"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
@@ -8413,8 +7351,8 @@
       <c r="L6" s="31"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
@@ -8427,8 +7365,8 @@
       <c r="L7" s="31"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
@@ -8441,8 +7379,8 @@
       <c r="L8" s="31"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
@@ -8455,8 +7393,8 @@
       <c r="L9" s="31"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="31"/>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
@@ -8469,8 +7407,8 @@
       <c r="L10" s="31"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
@@ -8483,8 +7421,8 @@
       <c r="L11" s="31"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
@@ -8497,8 +7435,8 @@
       <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
@@ -8511,8 +7449,8 @@
       <c r="L13" s="31"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -8525,8 +7463,8 @@
       <c r="L14" s="31"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -8539,8 +7477,8 @@
       <c r="L15" s="31"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
       <c r="E16" s="31"/>
@@ -8553,8 +7491,8 @@
       <c r="L16" s="31"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
       <c r="E17" s="31"/>
@@ -8567,8 +7505,8 @@
       <c r="L17" s="31"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
       <c r="E18" s="31"/>
@@ -8581,8 +7519,8 @@
       <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
@@ -8595,8 +7533,8 @@
       <c r="L19" s="31"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
@@ -8609,8 +7547,8 @@
       <c r="L20" s="31"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
@@ -8623,8 +7561,8 @@
       <c r="L21" s="31"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
@@ -8637,8 +7575,8 @@
       <c r="L22" s="31"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="63"/>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
@@ -8651,8 +7589,8 @@
       <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="63"/>
+      <c r="B24" s="63"/>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
       <c r="E24" s="31"/>
@@ -8665,8 +7603,8 @@
       <c r="L24" s="31"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
+      <c r="A25" s="63"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="31"/>
       <c r="D25" s="31"/>
       <c r="E25" s="31"/>
@@ -8679,8 +7617,8 @@
       <c r="L25" s="31"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
+      <c r="A26" s="63"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
@@ -8693,8 +7631,8 @@
       <c r="L26" s="31"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="63"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="31"/>
       <c r="D27" s="31"/>
       <c r="E27" s="31"/>
@@ -8707,8 +7645,8 @@
       <c r="L27" s="31"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
+      <c r="A28" s="63"/>
+      <c r="B28" s="63"/>
       <c r="C28" s="31"/>
       <c r="D28" s="31"/>
       <c r="E28" s="31"/>
@@ -8721,8 +7659,8 @@
       <c r="L28" s="31"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
+      <c r="A29" s="63"/>
+      <c r="B29" s="63"/>
       <c r="C29" s="31"/>
       <c r="D29" s="31"/>
       <c r="E29" s="31"/>
@@ -8735,8 +7673,8 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
+      <c r="A30" s="63"/>
+      <c r="B30" s="63"/>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
       <c r="E30" s="31"/>
@@ -8749,8 +7687,8 @@
       <c r="L30" s="31"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
+      <c r="A31" s="63"/>
+      <c r="B31" s="63"/>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
       <c r="E31" s="31"/>
@@ -8763,8 +7701,8 @@
       <c r="L31" s="31"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
+      <c r="A32" s="63"/>
+      <c r="B32" s="63"/>
       <c r="C32" s="31"/>
       <c r="D32" s="31"/>
       <c r="E32" s="31"/>
@@ -8777,8 +7715,8 @@
       <c r="L32" s="31"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
+      <c r="A33" s="63"/>
+      <c r="B33" s="63"/>
       <c r="C33" s="31"/>
       <c r="D33" s="31"/>
       <c r="E33" s="31"/>
@@ -8791,8 +7729,8 @@
       <c r="L33" s="31"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
+      <c r="A34" s="63"/>
+      <c r="B34" s="63"/>
       <c r="C34" s="31"/>
       <c r="D34" s="31"/>
       <c r="E34" s="31"/>
@@ -8805,8 +7743,8 @@
       <c r="L34" s="31"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
+      <c r="A35" s="63"/>
+      <c r="B35" s="63"/>
       <c r="C35" s="31"/>
       <c r="D35" s="31"/>
       <c r="E35" s="31"/>
@@ -8819,8 +7757,8 @@
       <c r="L35" s="31"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
+      <c r="A36" s="63"/>
+      <c r="B36" s="63"/>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
@@ -8833,8 +7771,8 @@
       <c r="L36" s="31"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
+      <c r="A37" s="63"/>
+      <c r="B37" s="63"/>
       <c r="C37" s="31"/>
       <c r="D37" s="31"/>
       <c r="E37" s="31"/>
@@ -8847,8 +7785,8 @@
       <c r="L37" s="31"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
+      <c r="A38" s="63"/>
+      <c r="B38" s="63"/>
       <c r="C38" s="31"/>
       <c r="D38" s="31"/>
       <c r="E38" s="31"/>
@@ -8861,8 +7799,8 @@
       <c r="L38" s="31"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
+      <c r="A39" s="63"/>
+      <c r="B39" s="63"/>
       <c r="C39" s="31"/>
       <c r="D39" s="31"/>
       <c r="E39" s="31"/>
@@ -8875,8 +7813,8 @@
       <c r="L39" s="31"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
+      <c r="A40" s="63"/>
+      <c r="B40" s="63"/>
       <c r="C40" s="31"/>
       <c r="D40" s="31"/>
       <c r="E40" s="31"/>
@@ -8889,8 +7827,8 @@
       <c r="L40" s="31"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
+      <c r="A41" s="63"/>
+      <c r="B41" s="63"/>
       <c r="C41" s="31"/>
       <c r="D41" s="31"/>
       <c r="E41" s="31"/>
@@ -8903,8 +7841,8 @@
       <c r="L41" s="31"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
+      <c r="A42" s="63"/>
+      <c r="B42" s="63"/>
       <c r="C42" s="31"/>
       <c r="D42" s="31"/>
       <c r="E42" s="31"/>
@@ -8917,8 +7855,8 @@
       <c r="L42" s="31"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31"/>
+      <c r="A43" s="63"/>
+      <c r="B43" s="63"/>
       <c r="C43" s="31"/>
       <c r="D43" s="31"/>
       <c r="E43" s="31"/>
@@ -8931,8 +7869,8 @@
       <c r="L43" s="31"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="63"/>
       <c r="C44" s="31"/>
       <c r="D44" s="31"/>
       <c r="E44" s="31"/>
@@ -8945,8 +7883,8 @@
       <c r="L44" s="31"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
+      <c r="A45" s="63"/>
+      <c r="B45" s="63"/>
       <c r="C45" s="31"/>
       <c r="D45" s="31"/>
       <c r="E45" s="31"/>
@@ -8959,8 +7897,8 @@
       <c r="L45" s="31"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="31"/>
       <c r="D46" s="31"/>
       <c r="E46" s="31"/>
@@ -8973,8 +7911,8 @@
       <c r="L46" s="31"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
+      <c r="A47" s="63"/>
+      <c r="B47" s="63"/>
       <c r="C47" s="31"/>
       <c r="D47" s="31"/>
       <c r="E47" s="31"/>
@@ -8987,8 +7925,8 @@
       <c r="L47" s="31"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
+      <c r="A48" s="63"/>
+      <c r="B48" s="63"/>
       <c r="C48" s="31"/>
       <c r="D48" s="31"/>
       <c r="E48" s="31"/>
@@ -9001,8 +7939,8 @@
       <c r="L48" s="31"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
+      <c r="A49" s="63"/>
+      <c r="B49" s="63"/>
       <c r="C49" s="31"/>
       <c r="D49" s="31"/>
       <c r="E49" s="31"/>
@@ -9015,8 +7953,8 @@
       <c r="L49" s="31"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
+      <c r="A50" s="63"/>
+      <c r="B50" s="63"/>
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
       <c r="E50" s="31"/>
@@ -9029,8 +7967,8 @@
       <c r="L50" s="31"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
+      <c r="A51" s="63"/>
+      <c r="B51" s="63"/>
       <c r="C51" s="31"/>
       <c r="D51" s="31"/>
       <c r="E51" s="31"/>
@@ -9052,7 +7990,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1803"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9071,7 +8011,7 @@
         <v>67</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>65</v>
@@ -9086,7 +8026,7 @@
         <v>77</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>70</v>
@@ -9115,7 +8055,7 @@
         <v>169</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F2" s="50" t="s">
         <v>173</v>
@@ -9124,7 +8064,7 @@
         <v>172</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I2" s="50" t="s">
         <v>211</v>
@@ -9133,10 +8073,10 @@
         <v>210</v>
       </c>
       <c r="K2" s="50" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="L2" s="50" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -27375,7 +26315,7 @@
         <v>67</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>65</v>
@@ -27390,7 +26330,7 @@
         <v>77</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>70</v>
@@ -27419,7 +26359,7 @@
         <v>169</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F2" s="50" t="s">
         <v>173</v>
@@ -27428,7 +26368,7 @@
         <v>172</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I2" s="50" t="s">
         <v>211</v>
@@ -27437,10 +26377,10 @@
         <v>210</v>
       </c>
       <c r="K2" s="50" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="L2" s="50" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -45683,7 +44623,7 @@
         <v>67</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>65</v>
@@ -45701,7 +44641,7 @@
         <v>70</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>66</v>
@@ -45727,7 +44667,7 @@
         <v>169</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F2" s="50" t="s">
         <v>173</v>
@@ -45739,16 +44679,16 @@
         <v>211</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J2" s="50" t="s">
         <v>210</v>
       </c>
       <c r="K2" s="50" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="L2" s="50" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -46504,7 +45444,7 @@
       </c>
       <c r="B3" s="67"/>
       <c r="E3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -46652,7 +45592,7 @@
       <c r="B3" s="22"/>
       <c r="C3" s="23"/>
       <c r="E3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -46985,7 +45925,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>85</v>
@@ -46996,83 +45936,83 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B2" s="59"/>
       <c r="D2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B3" s="60"/>
       <c r="D3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B4" s="60"/>
       <c r="D4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B5" s="59"/>
       <c r="D5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B6" s="60"/>
       <c r="D6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B7" s="60"/>
       <c r="D7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B8" s="60"/>
       <c r="D8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B9" s="60"/>
       <c r="D9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B10" s="61"/>
       <c r="D10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>